<commit_message>
suppr MS sur status
déjà en 1..1 17a18b45054cb726b06ab164b5f84aa00738fcd5
</commit_message>
<xml_diff>
--- a/sd-add_new-MS-questionnaire/ig/StructureDefinition-ror-questionnaire.xlsx
+++ b/sd-add_new-MS-questionnaire/ig/StructureDefinition-ror-questionnaire.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-10T14:17:45+00:00</t>
+    <t>2024-04-10T15:31:34+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -3942,7 +3942,7 @@
         <v>87</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="I17" t="s" s="2">
         <v>88</v>

</xml_diff>